<commit_message>
Exmet-II-Surfen: Excel data, protokol theory, Origin graph
</commit_message>
<xml_diff>
--- a/data/SurfenData.xlsx
+++ b/data/SurfenData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Surfenergy\Exmet-II-surfen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FAA6B8-2F0C-4A52-A679-1295EC8C01D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE665033-2084-4A98-95AE-27AC2F4BD897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="2745" windowWidth="19560" windowHeight="11385" xr2:uid="{3C3D8139-5023-48C2-AD43-8FCA81D0F4E0}"/>
+    <workbookView xWindow="17688" yWindow="2292" windowWidth="11580" windowHeight="12204" xr2:uid="{3C3D8139-5023-48C2-AD43-8FCA81D0F4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Voda</t>
   </si>
@@ -128,6 +128,51 @@
   </si>
   <si>
     <t>Li-Neumann</t>
+  </si>
+  <si>
+    <t>úhel [deg]</t>
+  </si>
+  <si>
+    <t>cos</t>
+  </si>
+  <si>
+    <t>úhel pm [deg]</t>
+  </si>
+  <si>
+    <t>kapalina</t>
+  </si>
+  <si>
+    <t>destilovaná voda</t>
+  </si>
+  <si>
+    <t>etylenglykol</t>
+  </si>
+  <si>
+    <t>dijodometan</t>
+  </si>
+  <si>
+    <t>glycerol</t>
+  </si>
+  <si>
+    <t>formamid</t>
+  </si>
+  <si>
+    <t>\gamma_l</t>
+  </si>
+  <si>
+    <t>\theta [deg]</t>
+  </si>
+  <si>
+    <t>pm \theta [deg]</t>
+  </si>
+  <si>
+    <t>cos \theta</t>
+  </si>
+  <si>
+    <t>pm cos \theta</t>
+  </si>
+  <si>
+    <t>relative pm</t>
   </si>
 </sst>
 </file>
@@ -175,11 +220,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -494,56 +539,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5169BA-CB8F-45DB-B13B-6D9A78F500B2}">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1" t="s">
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -614,7 +662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -652,7 +700,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -690,7 +738,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -728,7 +776,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -766,7 +814,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -804,7 +852,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -842,84 +890,93 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>5.67</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f>AVERAGEA(F3:F8)</f>
         <v>14.964999999999998</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f>SQRT(G3^2+G4^2+G5^2+G6^2+G7^2+G8^2)/COUNT(G3:G8)</f>
         <v>0.80425085915057892</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <f>SQRT(H3^2+H4^2+H5^2+H6^2+H7^2+H8^2)/COUNT(H3:H8)</f>
         <v>0.91177482600329196</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>18.96</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>3.06</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>3.06</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>21</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>3.73</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>10.85</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>22.1</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>1.08</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>1.08</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <f>AVERAGE(R3:R8)</f>
         <v>20.324999999999999</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <f>SQRT(S3^2+S4^2+S5^2+S6^2+S7^2+S8^2)/COUNT(S3:S8)</f>
         <v>0.86470772197572321</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="2">
         <f>SQRT(T3^2+T4^2+T5^2+T6^2+T7^2+T8^2)/COUNT(T3:T8)</f>
         <v>0.9269469000733298</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9" s="2">
         <f>AVERAGE(U3:U8)</f>
         <v>20.621666666666666</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="2">
         <f>SQRT(V3^2+V4^2+V5^2+V6^2+V7^2+V8^2)/COUNT(V3:V8)</f>
         <v>0.88556165479566962</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9" s="2">
         <f>SQRT(W3^2+W4^2+W5^2+W6^2+W7^2+W8^2)/COUNT(W3:W8)</f>
         <v>0.95218899851284189</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
       <c r="H10" t="s">
         <v>21</v>
       </c>
@@ -950,9 +1007,27 @@
       <c r="Q10">
         <v>0.91</v>
       </c>
-      <c r="T10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>102</v>
+      </c>
+      <c r="C11">
+        <f>COS(RADIANS(B11))</f>
+        <v>-0.20791169081775934</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>D11/B11</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="F11">
+        <f>E11*C11</f>
+        <v>-8.1533996399121306E-3</v>
+      </c>
       <c r="H11" t="s">
         <v>22</v>
       </c>
@@ -984,7 +1059,25 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C16" si="0">COS(RADIANS(B12))</f>
+        <v>3.489949670250108E-2</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E16" si="1">D12/B12</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F16" si="2">E12*C12</f>
+        <v>1.5863407592045947E-3</v>
+      </c>
       <c r="K12" t="s">
         <v>25</v>
       </c>
@@ -1007,7 +1100,25 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>77</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.22495105434386492</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>5.1948051948051951E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1.1685769056824152E-2</v>
+      </c>
       <c r="K13" t="s">
         <v>26</v>
       </c>
@@ -1028,6 +1139,281 @@
       </c>
       <c r="Q13">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>99</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-0.15643446504023081</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>-9.4808766691048974E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-1.7452406437283477E-2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>2.197802197802198E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>-3.8356937224798851E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.37460659341591196</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>4.4117647058823532E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>1.6526761474231412E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>72.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>58.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>102.4</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <f>COS(RADIANS(B27))</f>
+        <v>-0.2147353271670632</v>
+      </c>
+      <c r="E27">
+        <f>C27/B27</f>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="F27">
+        <f>E27*D27</f>
+        <v>-8.3880987174634065E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>88.1</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <f>COS(RADIANS(B28))</f>
+        <v>3.3155178388526496E-2</v>
+      </c>
+      <c r="E28">
+        <f>C28/B28</f>
+        <v>4.5402951191827474E-2</v>
+      </c>
+      <c r="F28">
+        <f>E28*D28</f>
+        <v>1.5053429461306016E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>76.7</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <f>COS(RADIANS(B29))</f>
+        <v>0.23004973718810445</v>
+      </c>
+      <c r="E29">
+        <f>C29/B29</f>
+        <v>5.2151238591916553E-2</v>
+      </c>
+      <c r="F29">
+        <f>E29*D29</f>
+        <v>1.1997378732104533E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>99.5</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <f>COS(RADIANS(B30))</f>
+        <v>-0.16504760586067771</v>
+      </c>
+      <c r="E30">
+        <f>C30/B30</f>
+        <v>6.030150753768844E-2</v>
+      </c>
+      <c r="F30">
+        <f>E30*D30</f>
+        <v>-9.9526194488850882E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>90.5</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <f>COS(RADIANS(B31))</f>
+        <v>-8.7265354983739971E-3</v>
+      </c>
+      <c r="E31">
+        <f>C31/B31</f>
+        <v>2.2099447513812154E-2</v>
+      </c>
+      <c r="F31">
+        <f>E31*D31</f>
+        <v>-1.9285161322373474E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>67.7</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <f>COS(RADIANS(B32))</f>
+        <v>0.37945615952900513</v>
+      </c>
+      <c r="E32">
+        <f>C32/B32</f>
+        <v>4.4313146233382568E-2</v>
+      </c>
+      <c r="F32">
+        <f>E32*D32</f>
+        <v>1.6814896286366548E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Surfen: Kwok a Li Neumann
</commit_message>
<xml_diff>
--- a/data/SurfenData.xlsx
+++ b/data/SurfenData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Surfenergy\Exmet-II-surfen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C69112-0E72-43BB-8A85-F4F3406A855D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F839BAF-BFA4-49C8-AF8A-6FCC37D10502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="4584" windowWidth="23040" windowHeight="12204" xr2:uid="{3C3D8139-5023-48C2-AD43-8FCA81D0F4E0}"/>
+    <workbookView xWindow="360" yWindow="3660" windowWidth="11076" windowHeight="12204" xr2:uid="{3C3D8139-5023-48C2-AD43-8FCA81D0F4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -346,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -374,7 +374,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -689,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5169BA-CB8F-45DB-B13B-6D9A78F500B2}">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,45 +707,46 @@
     <col min="5" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -803,17 +807,17 @@
       <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>16</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>17</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -846,16 +850,24 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="V3">
+        <f>AVERAGEA(T3:U3)</f>
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="W3">
         <v>21.59</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>1.69</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>2.58</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z3">
+        <f>AVERAGEA(X3:Y3)</f>
+        <v>2.1349999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -888,16 +900,24 @@
         <v>2.15</v>
       </c>
       <c r="V4">
+        <f t="shared" ref="V4:V16" si="1">AVERAGEA(T4:U4)</f>
+        <v>2.085</v>
+      </c>
+      <c r="W4">
         <v>16.420000000000002</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>2.0499999999999998</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>2.17</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z8" si="2">AVERAGEA(X4:Y4)</f>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -930,16 +950,24 @@
         <v>2.37</v>
       </c>
       <c r="V5">
+        <f t="shared" si="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="W5">
         <v>23.26</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1.91</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>2.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z5">
+        <f t="shared" si="2"/>
+        <v>2.1349999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -972,16 +1000,24 @@
         <v>3.3</v>
       </c>
       <c r="V6">
+        <f t="shared" si="1"/>
+        <v>3.36</v>
+      </c>
+      <c r="W6">
         <v>18.66</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>3.54</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z6">
+        <f t="shared" si="2"/>
+        <v>3.4850000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1014,16 +1050,24 @@
         <v>1.52</v>
       </c>
       <c r="V7">
+        <f t="shared" si="1"/>
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="W7">
         <v>20.29</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>1.56</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z7">
+        <f t="shared" si="2"/>
+        <v>1.5550000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1056,16 +1100,24 @@
         <v>1.26</v>
       </c>
       <c r="V8">
+        <f t="shared" si="1"/>
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="W8">
         <v>23.51</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>1.6</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z8">
+        <f t="shared" si="2"/>
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1133,20 +1185,28 @@
         <f>SQRT(U3^2+U4^2+U5^2+U6^2+U7^2+U8^2)/COUNT(U3:U8)</f>
         <v>0.9269469000733298</v>
       </c>
-      <c r="V9" s="2">
-        <f>AVERAGE(V3:V8)</f>
+      <c r="V9" s="1">
+        <f>_xlfn.STDEV.P(S3:S8)/SQRT(COUNT(S3:S8))</f>
+        <v>1.0355694890574276</v>
+      </c>
+      <c r="W9" s="2">
+        <f>AVERAGE(W3:W8)</f>
         <v>20.621666666666666</v>
-      </c>
-      <c r="W9" s="2">
-        <f>SQRT(W3^2+W4^2+W5^2+W6^2+W7^2+W8^2)/COUNT(W3:W8)</f>
-        <v>0.88556165479566962</v>
       </c>
       <c r="X9" s="2">
         <f>SQRT(X3^2+X4^2+X5^2+X6^2+X7^2+X8^2)/COUNT(X3:X8)</f>
+        <v>0.88556165479566962</v>
+      </c>
+      <c r="Y9" s="2">
+        <f>SQRT(Y3^2+Y4^2+Y5^2+Y6^2+Y7^2+Y8^2)/COUNT(Y3:Y8)</f>
         <v>0.95218899851284189</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z9" s="1">
+        <f>_xlfn.STDEV.P(W3:W8)/SQRT(COUNT(W3:W8))</f>
+        <v>1.0254143245717995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +1248,7 @@
       </c>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>102</v>
       </c>
@@ -1238,23 +1298,23 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>88</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C16" si="1">COS(RADIANS(B12))</f>
+        <f t="shared" ref="C12:C16" si="3">COS(RADIANS(B12))</f>
         <v>3.489949670250108E-2</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E16" si="2">D12/B12</f>
+        <f t="shared" ref="E12:E16" si="4">D12/B12</f>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F16" si="3">E12*C12</f>
+        <f t="shared" ref="F12:F16" si="5">E12*C12</f>
         <v>1.5863407592045947E-3</v>
       </c>
       <c r="L12" t="s">
@@ -1279,23 +1339,23 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>77</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.22495105434386492</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.1948051948051951E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1685769056824152E-2</v>
       </c>
       <c r="L13" t="s">
@@ -1320,63 +1380,63 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>99</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.15643446504023081</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.0606060606060608E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-9.4808766691048974E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>91</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1.7452406437283477E-2</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.197802197802198E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.8356937224798851E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>68</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.37460659341591196</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.4117647058823532E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.6526761474231412E-2</v>
       </c>
     </row>
@@ -1468,15 +1528,15 @@
         <v>4</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:D32" si="4">COS(RADIANS(B27))</f>
+        <f t="shared" ref="D27:D32" si="6">COS(RADIANS(B27))</f>
         <v>-0.2147353271670632</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E32" si="5">C27/B27</f>
+        <f t="shared" ref="E27:E32" si="7">C27/B27</f>
         <v>3.90625E-2</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:F32" si="6">E27*D27</f>
+        <f t="shared" ref="F27:F32" si="8">E27*D27</f>
         <v>-8.3880987174634065E-3</v>
       </c>
     </row>
@@ -1491,15 +1551,15 @@
         <v>4</v>
       </c>
       <c r="D28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3155178388526496E-2</v>
       </c>
       <c r="E28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.5402951191827474E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.5053429461306016E-3</v>
       </c>
     </row>
@@ -1514,15 +1574,15 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.23004973718810445</v>
       </c>
       <c r="E29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.2151238591916553E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1997378732104533E-2</v>
       </c>
     </row>
@@ -1537,15 +1597,15 @@
         <v>6</v>
       </c>
       <c r="D30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.16504760586067771</v>
       </c>
       <c r="E30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.030150753768844E-2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-9.9526194488850882E-3</v>
       </c>
     </row>
@@ -1560,15 +1620,15 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-8.7265354983739971E-3</v>
       </c>
       <c r="E31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.2099447513812154E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.9285161322373474E-4</v>
       </c>
     </row>
@@ -1583,15 +1643,15 @@
         <v>3</v>
       </c>
       <c r="D32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.37945615952900513</v>
       </c>
       <c r="E32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.4313146233382568E-2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.6814896286366548E-2</v>
       </c>
     </row>
@@ -1661,7 +1721,7 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="W1:Y1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="J1:L1"/>

</xml_diff>